<commit_message>
ticket 4336 - excel changes
git-svn-id: http://repos.luxurylink.com/svn/repos/toolbox/trunk@5552 bd3a7434-8174-4811-bcf6-7b9fed35a952
</commit_message>
<xml_diff>
--- a/app/views/packages/xls/Package.xlsx
+++ b/app/views/packages/xls/Package.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="46">
   <si>
     <t>%%LLTG_COMPANY_NAME%%</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Number of Guests:</t>
   </si>
   <si>
-    <t># of Children:</t>
-  </si>
-  <si>
     <t>Children Ages:</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
   </si>
   <si>
     <t>%%PACKAGE_FLEX_INFO%%</t>
-  </si>
-  <si>
-    <t>%%PACKAGE_NUM_CHILDREN%%</t>
   </si>
   <si>
     <t>%%PACKAGE_CHILDREN_AGES%%</t>
@@ -363,37 +357,37 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -699,10 +693,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A95" sqref="A95:XFD95"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -714,12 +708,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="31.5">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24"/>
+      <c r="B1" s="23"/>
       <c r="C1" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21">
@@ -744,760 +738,750 @@
       <c r="C5" s="27"/>
     </row>
     <row r="6" spans="1:3" s="6" customFormat="1" ht="23.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="21" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="21"/>
+      <c r="C7" s="28"/>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="21"/>
+      <c r="B8" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="28"/>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" s="28"/>
+      <c r="B9" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="29"/>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B10" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="29"/>
+        <v>36</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="30"/>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" s="21"/>
+      <c r="B11" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="28"/>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B12" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="21"/>
+        <v>41</v>
+      </c>
+      <c r="B12" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="28"/>
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="21"/>
+      <c r="B13" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="28"/>
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="21" t="s">
+      <c r="B14" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="28"/>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="21"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="21"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="21"/>
-    </row>
-    <row r="17" spans="1:3" s="6" customFormat="1" ht="23.25">
-      <c r="A17" s="22" t="s">
+      <c r="C15" s="28"/>
+    </row>
+    <row r="16" spans="1:3" s="6" customFormat="1" ht="23.25">
+      <c r="A16" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="B19" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="22"/>
-      <c r="C17" s="22"/>
-    </row>
-    <row r="18" spans="1:3">
-      <c r="A18" s="20" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3">
-      <c r="A19" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="18">
+        <f>SUM(C18:C18)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="23.25">
+      <c r="A21" s="24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
-      <c r="B20" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C20" s="18">
-        <f>SUM(C19:C19)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="23.25">
-      <c r="A22" s="22" t="s">
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="22"/>
-      <c r="C22" s="22"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
     </row>
     <row r="23" spans="1:3">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+    </row>
+    <row r="24" spans="1:3" ht="23.25">
+      <c r="A24" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-    </row>
-    <row r="24" spans="1:3">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-    </row>
-    <row r="25" spans="1:3" ht="23.25">
-      <c r="A25" s="22" t="s">
-        <v>41</v>
-      </c>
-      <c r="B25" s="22"/>
-      <c r="C25" s="22"/>
-    </row>
-    <row r="26" spans="1:3">
-      <c r="A26" s="23" t="s">
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+    </row>
+    <row r="27" spans="1:3" ht="23.25">
+      <c r="A27" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-    </row>
-    <row r="28" spans="1:3" ht="23.25">
-      <c r="A28" s="22" t="s">
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="22"/>
-      <c r="C28" s="22"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-    </row>
-    <row r="31" spans="1:3" s="31" customFormat="1" ht="23.25">
-      <c r="A31" s="30" t="s">
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+    </row>
+    <row r="30" spans="1:3" s="21" customFormat="1" ht="23.25">
+      <c r="A30" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="14"/>
     </row>
     <row r="32" spans="1:3">
       <c r="A32" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="B32" s="4"/>
+      <c r="C32" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="33" spans="1:3">
       <c r="A33" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B33" s="13">
+        <f>B32*C33</f>
+        <v>0</v>
+      </c>
+      <c r="C33" s="11"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" s="13">
-        <f>B33*C34</f>
-        <v>0</v>
-      </c>
-      <c r="C34" s="11"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="12" t="str">
+        <f>IF(B32=0,"",B34/B32)</f>
+        <v/>
+      </c>
     </row>
     <row r="35" spans="1:3">
       <c r="A35" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="12" t="str">
-        <f>IF(B33=0,"",B35/B33)</f>
+        <f>IF(B32=0,"",B35/B32)</f>
         <v/>
       </c>
     </row>
     <row r="36" spans="1:3">
       <c r="A36" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B36" s="4"/>
-      <c r="C36" s="12" t="str">
-        <f>IF(B33=0,"",B36/B33)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="12"/>
-    </row>
-    <row r="39" spans="1:3" s="31" customFormat="1" ht="23.25">
-      <c r="A39" s="30" t="s">
+      <c r="C36" s="12"/>
+    </row>
+    <row r="38" spans="1:3" s="21" customFormat="1" ht="23.25">
+      <c r="A38" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="14"/>
     </row>
     <row r="40" spans="1:3">
       <c r="A40" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="B40" s="4"/>
+      <c r="C40" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41" s="13">
+        <f>B40*C41</f>
+        <v>0</v>
+      </c>
+      <c r="C41" s="11"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B41" s="4"/>
-      <c r="C41" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B42" s="13">
-        <f>B41*C42</f>
-        <v>0</v>
-      </c>
-      <c r="C42" s="11"/>
+      <c r="B42" s="4"/>
+      <c r="C42" s="12" t="str">
+        <f>IF(B40=0,"",B42/B40)</f>
+        <v/>
+      </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="12" t="str">
-        <f>IF(B41=0,"",B43/B41)</f>
+        <f>IF(B40=0,"",B43/B40)</f>
         <v/>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B44" s="4"/>
-      <c r="C44" s="12" t="str">
-        <f>IF(B41=0,"",B44/B41)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B45" s="4"/>
-      <c r="C45" s="12"/>
-    </row>
-    <row r="47" spans="1:3" s="31" customFormat="1" ht="23.25">
-      <c r="A47" s="30" t="s">
+      <c r="C44" s="12"/>
+    </row>
+    <row r="46" spans="1:3" s="21" customFormat="1" ht="23.25">
+      <c r="A46" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B46" s="22"/>
+      <c r="C46" s="22"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B47" s="30"/>
-      <c r="C47" s="30"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="14"/>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="B48" s="4"/>
+      <c r="C48" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B49" s="13">
+        <f>B48*C49</f>
+        <v>0</v>
+      </c>
+      <c r="C49" s="11"/>
+    </row>
+    <row r="50" spans="1:3">
+      <c r="A50" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B49" s="4"/>
-      <c r="C49" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B50" s="13">
-        <f>B49*C50</f>
-        <v>0</v>
-      </c>
-      <c r="C50" s="11"/>
+      <c r="B50" s="4"/>
+      <c r="C50" s="12" t="str">
+        <f>IF(B48=0,"",B50/B48)</f>
+        <v/>
+      </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="12" t="str">
-        <f>IF(B49=0,"",B51/B49)</f>
+        <f>IF(B48=0,"",B51/B48)</f>
         <v/>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="A52" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B52" s="4"/>
-      <c r="C52" s="12" t="str">
-        <f>IF(B49=0,"",B52/B49)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B53" s="4"/>
-      <c r="C53" s="12"/>
-    </row>
-    <row r="55" spans="1:3" s="31" customFormat="1" ht="23.25">
-      <c r="A55" s="30" t="s">
+      <c r="C52" s="12"/>
+    </row>
+    <row r="54" spans="1:3" s="21" customFormat="1" ht="23.25">
+      <c r="A54" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B54" s="22"/>
+      <c r="C54" s="22"/>
+    </row>
+    <row r="55" spans="1:3">
+      <c r="A55" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B55" s="30"/>
-      <c r="C55" s="30"/>
+      <c r="B55" s="17"/>
+      <c r="C55" s="14"/>
     </row>
     <row r="56" spans="1:3">
       <c r="A56" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B56" s="17"/>
-      <c r="C56" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="B56" s="4"/>
+      <c r="C56" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B57" s="13">
+        <f>B56*C57</f>
+        <v>0</v>
+      </c>
+      <c r="C57" s="11"/>
+    </row>
+    <row r="58" spans="1:3">
+      <c r="A58" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B57" s="4"/>
-      <c r="C57" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B58" s="13">
-        <f>B57*C58</f>
-        <v>0</v>
-      </c>
-      <c r="C58" s="11"/>
+      <c r="B58" s="4"/>
+      <c r="C58" s="12" t="str">
+        <f>IF(B56=0,"",B58/B56)</f>
+        <v/>
+      </c>
     </row>
     <row r="59" spans="1:3">
       <c r="A59" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B59" s="4"/>
       <c r="C59" s="12" t="str">
-        <f>IF(B57=0,"",B59/B57)</f>
+        <f>IF(B56=0,"",B59/B56)</f>
         <v/>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="A60" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B60" s="4"/>
-      <c r="C60" s="12" t="str">
-        <f>IF(B57=0,"",B60/B57)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B61" s="4"/>
-      <c r="C61" s="12"/>
-    </row>
-    <row r="63" spans="1:3" s="31" customFormat="1" ht="23.25">
-      <c r="A63" s="30" t="s">
+      <c r="C60" s="12"/>
+    </row>
+    <row r="62" spans="1:3" s="21" customFormat="1" ht="23.25">
+      <c r="A62" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B62" s="22"/>
+      <c r="C62" s="22"/>
+    </row>
+    <row r="63" spans="1:3">
+      <c r="A63" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B63" s="30"/>
-      <c r="C63" s="30"/>
+      <c r="B63" s="17"/>
+      <c r="C63" s="14"/>
     </row>
     <row r="64" spans="1:3">
       <c r="A64" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B64" s="17"/>
-      <c r="C64" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="B64" s="4"/>
+      <c r="C64" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="65" spans="1:3">
       <c r="A65" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B65" s="13">
+        <f>B64*C65</f>
+        <v>0</v>
+      </c>
+      <c r="C65" s="11"/>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B65" s="4"/>
-      <c r="C65" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B66" s="13">
-        <f>B65*C66</f>
-        <v>0</v>
-      </c>
-      <c r="C66" s="11"/>
+      <c r="B66" s="4"/>
+      <c r="C66" s="12" t="str">
+        <f>IF(B64=0,"",B66/B64)</f>
+        <v/>
+      </c>
     </row>
     <row r="67" spans="1:3">
       <c r="A67" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="12" t="str">
-        <f>IF(B65=0,"",B67/B65)</f>
+        <f>IF(B64=0,"",B67/B64)</f>
         <v/>
       </c>
     </row>
     <row r="68" spans="1:3">
       <c r="A68" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B68" s="4"/>
-      <c r="C68" s="12" t="str">
-        <f>IF(B65=0,"",B68/B65)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B69" s="4"/>
-      <c r="C69" s="12"/>
-    </row>
-    <row r="71" spans="1:3" s="31" customFormat="1" ht="23.25">
-      <c r="A71" s="30" t="s">
+      <c r="C68" s="12"/>
+    </row>
+    <row r="70" spans="1:3" s="21" customFormat="1" ht="23.25">
+      <c r="A70" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B70" s="22"/>
+      <c r="C70" s="22"/>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B71" s="30"/>
-      <c r="C71" s="30"/>
+      <c r="B71" s="17"/>
+      <c r="C71" s="14"/>
     </row>
     <row r="72" spans="1:3">
       <c r="A72" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B72" s="17"/>
-      <c r="C72" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="B72" s="4"/>
+      <c r="C72" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="73" spans="1:3">
       <c r="A73" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B73" s="13">
+        <f>B72*C73</f>
+        <v>0</v>
+      </c>
+      <c r="C73" s="11"/>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B73" s="4"/>
-      <c r="C73" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B74" s="13">
-        <f>B73*C74</f>
-        <v>0</v>
-      </c>
-      <c r="C74" s="11"/>
+      <c r="B74" s="4"/>
+      <c r="C74" s="12" t="str">
+        <f>IF(B72=0,"",B74/B72)</f>
+        <v/>
+      </c>
     </row>
     <row r="75" spans="1:3">
       <c r="A75" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B75" s="4"/>
       <c r="C75" s="12" t="str">
-        <f>IF(B73=0,"",B75/B73)</f>
+        <f>IF(B72=0,"",B75/B72)</f>
         <v/>
       </c>
     </row>
     <row r="76" spans="1:3">
       <c r="A76" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B76" s="4"/>
-      <c r="C76" s="12" t="str">
-        <f>IF(B73=0,"",B76/B73)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B77" s="4"/>
-      <c r="C77" s="12"/>
-    </row>
-    <row r="79" spans="1:3" s="31" customFormat="1" ht="23.25">
-      <c r="A79" s="30" t="s">
+      <c r="C76" s="12"/>
+    </row>
+    <row r="78" spans="1:3" s="21" customFormat="1" ht="23.25">
+      <c r="A78" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B78" s="22"/>
+      <c r="C78" s="22"/>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B79" s="30"/>
-      <c r="C79" s="30"/>
+      <c r="B79" s="17"/>
+      <c r="C79" s="14"/>
     </row>
     <row r="80" spans="1:3">
       <c r="A80" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B80" s="17"/>
-      <c r="C80" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="B80" s="4"/>
+      <c r="C80" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="81" spans="1:3">
       <c r="A81" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B81" s="13">
+        <f>B80*C81</f>
+        <v>0</v>
+      </c>
+      <c r="C81" s="11"/>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B81" s="4"/>
-      <c r="C81" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B82" s="13">
-        <f>B81*C82</f>
-        <v>0</v>
-      </c>
-      <c r="C82" s="11"/>
+      <c r="B82" s="4"/>
+      <c r="C82" s="12" t="str">
+        <f>IF(B80=0,"",B82/B80)</f>
+        <v/>
+      </c>
     </row>
     <row r="83" spans="1:3">
       <c r="A83" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B83" s="4"/>
       <c r="C83" s="12" t="str">
-        <f>IF(B81=0,"",B83/B81)</f>
+        <f>IF(B80=0,"",B83/B80)</f>
         <v/>
       </c>
     </row>
     <row r="84" spans="1:3">
       <c r="A84" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B84" s="4"/>
-      <c r="C84" s="12" t="str">
-        <f>IF(B81=0,"",B84/B81)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B85" s="4"/>
-      <c r="C85" s="12"/>
-    </row>
-    <row r="87" spans="1:3" s="31" customFormat="1" ht="23.25">
-      <c r="A87" s="30" t="s">
+      <c r="C84" s="12"/>
+    </row>
+    <row r="86" spans="1:3" s="21" customFormat="1" ht="23.25">
+      <c r="A86" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B86" s="22"/>
+      <c r="C86" s="22"/>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B87" s="30"/>
-      <c r="C87" s="30"/>
+      <c r="B87" s="17"/>
+      <c r="C87" s="14"/>
     </row>
     <row r="88" spans="1:3">
       <c r="A88" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B88" s="17"/>
-      <c r="C88" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="B88" s="4"/>
+      <c r="C88" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="89" spans="1:3">
       <c r="A89" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B89" s="13">
+        <f>B88*C89</f>
+        <v>0</v>
+      </c>
+      <c r="C89" s="11"/>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B89" s="4"/>
-      <c r="C89" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B90" s="13">
-        <f>B89*C90</f>
-        <v>0</v>
-      </c>
-      <c r="C90" s="11"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="12" t="str">
+        <f>IF(B88=0,"",B90/B88)</f>
+        <v/>
+      </c>
     </row>
     <row r="91" spans="1:3">
       <c r="A91" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B91" s="4"/>
       <c r="C91" s="12" t="str">
-        <f>IF(B89=0,"",B91/B89)</f>
+        <f>IF(B88=0,"",B91/B88)</f>
         <v/>
       </c>
     </row>
     <row r="92" spans="1:3">
       <c r="A92" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B92" s="4"/>
-      <c r="C92" s="12" t="str">
-        <f>IF(B89=0,"",B92/B89)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B93" s="4"/>
-      <c r="C93" s="12"/>
-    </row>
-    <row r="95" spans="1:3" s="31" customFormat="1" ht="23.25">
-      <c r="A95" s="30" t="s">
+      <c r="C92" s="12"/>
+    </row>
+    <row r="94" spans="1:3" s="21" customFormat="1" ht="23.25">
+      <c r="A94" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B94" s="22"/>
+      <c r="C94" s="22"/>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B95" s="30"/>
-      <c r="C95" s="30"/>
+      <c r="B95" s="17"/>
+      <c r="C95" s="14"/>
     </row>
     <row r="96" spans="1:3">
       <c r="A96" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B96" s="17"/>
-      <c r="C96" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="B96" s="4"/>
+      <c r="C96" s="7" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="97" spans="1:3">
       <c r="A97" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B97" s="13">
+        <f>B96*C97</f>
+        <v>0</v>
+      </c>
+      <c r="C97" s="11"/>
+    </row>
+    <row r="98" spans="1:3">
+      <c r="A98" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B97" s="4"/>
-      <c r="C97" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B98" s="13">
-        <f>B97*C98</f>
-        <v>0</v>
-      </c>
-      <c r="C98" s="11"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="12" t="str">
+        <f>IF(B96=0,"",B98/B96)</f>
+        <v/>
+      </c>
     </row>
     <row r="99" spans="1:3">
       <c r="A99" s="2" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="B99" s="4"/>
       <c r="C99" s="12" t="str">
-        <f>IF(B97=0,"",B99/B97)</f>
+        <f>IF(B96=0,"",B99/B96)</f>
         <v/>
       </c>
     </row>
     <row r="100" spans="1:3">
       <c r="A100" s="2" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B100" s="4"/>
-      <c r="C100" s="12" t="str">
-        <f>IF(B97=0,"",B100/B97)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="101" spans="1:3">
-      <c r="A101" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B101" s="4"/>
-      <c r="C101" s="12"/>
+      <c r="C100" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="31">
-    <mergeCell ref="A63:C63"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="A79:C79"/>
-    <mergeCell ref="A87:C87"/>
-    <mergeCell ref="A95:C95"/>
+  <mergeCells count="30">
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="A30:C30"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A54:C54"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="A28:C28"/>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A21:C21"/>
     <mergeCell ref="A3:C3"/>
     <mergeCell ref="A4:C4"/>
     <mergeCell ref="A5:C5"/>
     <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A16:C16"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A26:C26"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A47:C47"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A78:C78"/>
+    <mergeCell ref="A86:C86"/>
+    <mergeCell ref="A94:C94"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
TICKET4625: moved excel fields around
git-svn-id: http://repos.luxurylink.com/svn/repos/toolbox/trunk@5917 bd3a7434-8174-4811-bcf6-7b9fed35a952
</commit_message>
<xml_diff>
--- a/app/views/packages/xls/Package.xlsx
+++ b/app/views/packages/xls/Package.xlsx
@@ -381,12 +381,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -396,20 +405,11 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -719,8 +719,8 @@
   </sheetPr>
   <dimension ref="A1:C152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A130" sqref="A130:C130"/>
+    <sheetView tabSelected="1" topLeftCell="A118" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G138" sqref="G138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,129 +732,129 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.5">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
+      <c r="B1" s="29"/>
       <c r="C1" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
     </row>
     <row r="4" spans="1:3" s="9" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="28" t="s">
+      <c r="A4" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
     </row>
     <row r="5" spans="1:3" s="8" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="29"/>
-      <c r="C5" s="29"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
     </row>
     <row r="6" spans="1:3" s="6" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A6" s="26" t="s">
+      <c r="A6" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="26"/>
-      <c r="C6" s="26"/>
+      <c r="B6" s="28"/>
+      <c r="C6" s="28"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="30"/>
+      <c r="C7" s="25"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="30"/>
+      <c r="C8" s="25"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="31"/>
+      <c r="C9" s="33"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="32"/>
+      <c r="C10" s="34"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="30"/>
+      <c r="C11" s="25"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="30"/>
+      <c r="C12" s="25"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="30"/>
+      <c r="C13" s="25"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="C14" s="30"/>
+      <c r="C14" s="25"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="30"/>
+      <c r="C15" s="25"/>
     </row>
     <row r="16" spans="1:3" s="6" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A16" s="26" t="s">
+      <c r="A16" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
+      <c r="B16" s="28"/>
+      <c r="C16" s="28"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
@@ -888,18 +888,18 @@
       </c>
     </row>
     <row r="21" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="34" t="s">
+      <c r="A22" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="34"/>
-      <c r="C22" s="34"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="15"/>
@@ -907,39 +907,39 @@
       <c r="C23" s="15"/>
     </row>
     <row r="24" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A24" s="26" t="s">
+      <c r="A24" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="34" t="s">
+      <c r="A25" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="34"/>
-      <c r="C25" s="34"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="27"/>
     </row>
     <row r="27" spans="1:3" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A27" s="26" t="s">
+      <c r="A27" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="34" t="s">
+      <c r="A28" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B28" s="34"/>
-      <c r="C28" s="34"/>
+      <c r="B28" s="27"/>
+      <c r="C28" s="27"/>
     </row>
     <row r="30" spans="1:3" s="21" customFormat="1" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A30" s="33" t="s">
+      <c r="A30" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="33"/>
-      <c r="C30" s="33"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
     </row>
     <row r="31" spans="1:3" s="21" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="s">
@@ -950,74 +950,74 @@
     </row>
     <row r="32" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B32" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="B32" s="22"/>
       <c r="C32" s="14"/>
     </row>
-    <row r="33" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="22"/>
+        <v>31</v>
+      </c>
+      <c r="B33" s="17"/>
       <c r="C33" s="14"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="17"/>
-      <c r="C34" s="14"/>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="B34" s="4"/>
+      <c r="C34" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B35" s="4"/>
-      <c r="C35" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="C35" s="14"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="4"/>
+      <c r="C36" s="12"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B36" s="13">
-        <f>B35*C36</f>
+      <c r="B37" s="13">
+        <f>B34*C37</f>
         <v>0</v>
       </c>
-      <c r="C36" s="11"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="12" t="str">
-        <f>IF(B35=0,"",B37/B35)</f>
-        <v/>
-      </c>
+      <c r="C37" s="11"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B38" s="4"/>
       <c r="C38" s="12" t="str">
-        <f>IF(B35=0,"",B38/B35)</f>
+        <f>IF(B34=0,"",B38/B34)</f>
         <v/>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B39" s="4"/>
-      <c r="C39" s="12"/>
+      <c r="C39" s="12" t="str">
+        <f>IF(B34=0,"",B39/B34)</f>
+        <v/>
+      </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="12"/>
@@ -1031,74 +1031,74 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="B43" s="22"/>
       <c r="C43" s="14"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B44" s="22"/>
+        <v>31</v>
+      </c>
+      <c r="B44" s="17"/>
       <c r="C44" s="14"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B45" s="17"/>
-      <c r="C45" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="B45" s="4"/>
+      <c r="C45" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B46" s="4"/>
-      <c r="C46" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="C46" s="14"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="12"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="13">
-        <f>B46*C47</f>
+      <c r="B48" s="13">
+        <f>B45*C48</f>
         <v>0</v>
       </c>
-      <c r="C47" s="11"/>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B48" s="4"/>
-      <c r="C48" s="12" t="str">
-        <f>IF(B46=0,"",B48/B46)</f>
-        <v/>
-      </c>
+      <c r="C48" s="11"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="12" t="str">
-        <f>IF(B46=0,"",B49/B46)</f>
+        <f>IF(B45=0,"",B49/B45)</f>
         <v/>
       </c>
     </row>
     <row r="50" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B50" s="4"/>
-      <c r="C50" s="12"/>
+      <c r="C50" s="12" t="str">
+        <f>IF(B45=0,"",B50/B45)</f>
+        <v/>
+      </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="12"/>
@@ -1112,74 +1112,74 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B54" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="B54" s="22"/>
       <c r="C54" s="14"/>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B55" s="22"/>
+        <v>31</v>
+      </c>
+      <c r="B55" s="17"/>
       <c r="C55" s="14"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B56" s="17"/>
-      <c r="C56" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="B56" s="4"/>
+      <c r="C56" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B57" s="4"/>
-      <c r="C57" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="C57" s="14"/>
     </row>
     <row r="58" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B58" s="4"/>
+      <c r="C58" s="12"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B58" s="13">
-        <f>B57*C58</f>
+      <c r="B59" s="13">
+        <f>B56*C59</f>
         <v>0</v>
       </c>
-      <c r="C58" s="11"/>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B59" s="4"/>
-      <c r="C59" s="12" t="str">
-        <f>IF(B57=0,"",B59/B57)</f>
-        <v/>
-      </c>
+      <c r="C59" s="11"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B60" s="4"/>
       <c r="C60" s="12" t="str">
-        <f>IF(B57=0,"",B60/B57)</f>
+        <f>IF(B56=0,"",B60/B56)</f>
         <v/>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B61" s="4"/>
-      <c r="C61" s="12"/>
+      <c r="C61" s="12" t="str">
+        <f>IF(B56=0,"",B61/B56)</f>
+        <v/>
+      </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B62" s="4"/>
       <c r="C62" s="12"/>
@@ -1193,74 +1193,74 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B65" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="B65" s="22"/>
       <c r="C65" s="14"/>
     </row>
     <row r="66" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B66" s="22"/>
+        <v>31</v>
+      </c>
+      <c r="B66" s="17"/>
       <c r="C66" s="14"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B67" s="17"/>
-      <c r="C67" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="B67" s="4"/>
+      <c r="C67" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B68" s="4"/>
-      <c r="C68" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="C68" s="14"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B69" s="4"/>
+      <c r="C69" s="12"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B69" s="13">
-        <f>B68*C69</f>
+      <c r="B70" s="13">
+        <f>B67*C70</f>
         <v>0</v>
       </c>
-      <c r="C69" s="11"/>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B70" s="4"/>
-      <c r="C70" s="12" t="str">
-        <f>IF(B68=0,"",B70/B68)</f>
-        <v/>
-      </c>
+      <c r="C70" s="11"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B71" s="4"/>
       <c r="C71" s="12" t="str">
-        <f>IF(B68=0,"",B71/B68)</f>
+        <f>IF(B67=0,"",B71/B67)</f>
         <v/>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B72" s="4"/>
-      <c r="C72" s="12"/>
+      <c r="C72" s="12" t="str">
+        <f>IF(B67=0,"",B72/B67)</f>
+        <v/>
+      </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="12"/>
@@ -1279,74 +1279,74 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B76" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="B76" s="22"/>
       <c r="C76" s="14"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B77" s="22"/>
+        <v>31</v>
+      </c>
+      <c r="B77" s="17"/>
       <c r="C77" s="14"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B78" s="17"/>
-      <c r="C78" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="B78" s="4"/>
+      <c r="C78" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B79" s="4"/>
-      <c r="C79" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="C79" s="14"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B80" s="4"/>
+      <c r="C80" s="12"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B80" s="13">
-        <f>B79*C80</f>
+      <c r="B81" s="13">
+        <f>B78*C81</f>
         <v>0</v>
       </c>
-      <c r="C80" s="11"/>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B81" s="4"/>
-      <c r="C81" s="12" t="str">
-        <f>IF(B79=0,"",B81/B79)</f>
-        <v/>
-      </c>
+      <c r="C81" s="11"/>
     </row>
     <row r="82" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="12" t="str">
-        <f>IF(B79=0,"",B82/B79)</f>
+        <f>IF(B78=0,"",B82/B78)</f>
         <v/>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B83" s="4"/>
-      <c r="C83" s="12"/>
+      <c r="C83" s="12" t="str">
+        <f>IF(B78=0,"",B83/B78)</f>
+        <v/>
+      </c>
     </row>
     <row r="84" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B84" s="4"/>
       <c r="C84" s="12"/>
@@ -1360,74 +1360,74 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B87" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="B87" s="22"/>
       <c r="C87" s="14"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B88" s="22"/>
+        <v>31</v>
+      </c>
+      <c r="B88" s="17"/>
       <c r="C88" s="14"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B89" s="17"/>
-      <c r="C89" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="B89" s="4"/>
+      <c r="C89" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="90" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B90" s="4"/>
-      <c r="C90" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="C90" s="14"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
+      <c r="A91" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B91" s="4"/>
+      <c r="C91" s="12"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B91" s="13">
-        <f>B90*C91</f>
+      <c r="B92" s="13">
+        <f>B89*C92</f>
         <v>0</v>
       </c>
-      <c r="C91" s="11"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B92" s="4"/>
-      <c r="C92" s="12" t="str">
-        <f>IF(B90=0,"",B92/B90)</f>
-        <v/>
-      </c>
+      <c r="C92" s="11"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B93" s="4"/>
       <c r="C93" s="12" t="str">
-        <f>IF(B90=0,"",B93/B90)</f>
+        <f>IF(B89=0,"",B93/B89)</f>
         <v/>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B94" s="4"/>
-      <c r="C94" s="12"/>
+      <c r="C94" s="12" t="str">
+        <f>IF(B89=0,"",B94/B89)</f>
+        <v/>
+      </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B95" s="4"/>
       <c r="C95" s="12"/>
@@ -1439,76 +1439,76 @@
       <c r="B97" s="24"/>
       <c r="C97" s="24"/>
     </row>
-    <row r="98" spans="1:3" s="21" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B98" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="B98" s="22"/>
       <c r="C98" s="14"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B99" s="22"/>
+        <v>31</v>
+      </c>
+      <c r="B99" s="17"/>
       <c r="C99" s="14"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B100" s="17"/>
-      <c r="C100" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="B100" s="4"/>
+      <c r="C100" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B101" s="4"/>
-      <c r="C101" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="C101" s="14"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+      <c r="A102" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B102" s="4"/>
+      <c r="C102" s="12"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B102" s="13">
-        <f>B101*C102</f>
+      <c r="B103" s="13">
+        <f>B100*C103</f>
         <v>0</v>
       </c>
-      <c r="C102" s="11"/>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B103" s="4"/>
-      <c r="C103" s="12" t="str">
-        <f>IF(B101=0,"",B103/B101)</f>
-        <v/>
-      </c>
+      <c r="C103" s="11"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B104" s="4"/>
       <c r="C104" s="12" t="str">
-        <f>IF(B101=0,"",B104/B101)</f>
+        <f>IF(B100=0,"",B104/B100)</f>
         <v/>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B105" s="4"/>
-      <c r="C105" s="12"/>
+      <c r="C105" s="12" t="str">
+        <f>IF(B100=0,"",B105/B100)</f>
+        <v/>
+      </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B106" s="4"/>
       <c r="C106" s="12"/>
@@ -1522,74 +1522,74 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B109" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="B109" s="22"/>
       <c r="C109" s="14"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B110" s="22"/>
+        <v>31</v>
+      </c>
+      <c r="B110" s="17"/>
       <c r="C110" s="14"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B111" s="17"/>
-      <c r="C111" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="B111" s="4"/>
+      <c r="C111" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B112" s="4"/>
-      <c r="C112" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="C112" s="14"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+      <c r="A113" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B113" s="4"/>
+      <c r="C113" s="12"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B113" s="13">
-        <f>B112*C113</f>
+      <c r="B114" s="13">
+        <f>B111*C114</f>
         <v>0</v>
       </c>
-      <c r="C113" s="11"/>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B114" s="4"/>
-      <c r="C114" s="12" t="str">
-        <f>IF(B112=0,"",B114/B112)</f>
-        <v/>
-      </c>
+      <c r="C114" s="11"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B115" s="4"/>
       <c r="C115" s="12" t="str">
-        <f>IF(B112=0,"",B115/B112)</f>
+        <f>IF(B111=0,"",B115/B111)</f>
         <v/>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B116" s="4"/>
-      <c r="C116" s="12"/>
+      <c r="C116" s="12" t="str">
+        <f>IF(B111=0,"",B116/B111)</f>
+        <v/>
+      </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B117" s="4"/>
       <c r="C117" s="12"/>
@@ -1603,74 +1603,74 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B120" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="B120" s="22"/>
       <c r="C120" s="14"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B121" s="22"/>
+        <v>31</v>
+      </c>
+      <c r="B121" s="17"/>
       <c r="C121" s="14"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B122" s="17"/>
-      <c r="C122" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="B122" s="4"/>
+      <c r="C122" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B123" s="4"/>
-      <c r="C123" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="C123" s="14"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
+      <c r="A124" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B124" s="4"/>
+      <c r="C124" s="12"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B124" s="13">
-        <f>B123*C124</f>
+      <c r="B125" s="13">
+        <f>B122*C125</f>
         <v>0</v>
       </c>
-      <c r="C124" s="11"/>
-    </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B125" s="4"/>
-      <c r="C125" s="12" t="str">
-        <f>IF(B123=0,"",B125/B123)</f>
-        <v/>
-      </c>
+      <c r="C125" s="11"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B126" s="4"/>
       <c r="C126" s="12" t="str">
-        <f>IF(B123=0,"",B126/B123)</f>
+        <f>IF(B122=0,"",B126/B122)</f>
         <v/>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B127" s="4"/>
-      <c r="C127" s="12"/>
+      <c r="C127" s="12" t="str">
+        <f>IF(B122=0,"",B127/B122)</f>
+        <v/>
+      </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B128" s="4"/>
       <c r="C128" s="12"/>
@@ -1684,74 +1684,74 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B131" s="4"/>
+        <v>45</v>
+      </c>
+      <c r="B131" s="22"/>
       <c r="C131" s="14"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B132" s="22"/>
+        <v>31</v>
+      </c>
+      <c r="B132" s="17"/>
       <c r="C132" s="14"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B133" s="17"/>
-      <c r="C133" s="14"/>
+        <v>27</v>
+      </c>
+      <c r="B133" s="4"/>
+      <c r="C133" s="7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B134" s="4"/>
-      <c r="C134" s="7" t="s">
-        <v>29</v>
-      </c>
+      <c r="C134" s="14"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
+      <c r="A135" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B135" s="4"/>
+      <c r="C135" s="12"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B135" s="13">
-        <f>B134*C135</f>
+      <c r="B136" s="13">
+        <f>B133*C136</f>
         <v>0</v>
       </c>
-      <c r="C135" s="11"/>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A136" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B136" s="4"/>
-      <c r="C136" s="12" t="str">
-        <f>IF(B134=0,"",B136/B134)</f>
-        <v/>
-      </c>
+      <c r="C136" s="11"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B137" s="4"/>
       <c r="C137" s="12" t="str">
-        <f>IF(B134=0,"",B137/B134)</f>
+        <f>IF(B133=0,"",B137/B133)</f>
         <v/>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="B138" s="4"/>
-      <c r="C138" s="12"/>
+      <c r="C138" s="12" t="str">
+        <f>IF(B133=0,"",B138/B133)</f>
+        <v/>
+      </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B139" s="4"/>
       <c r="C139" s="12"/>
@@ -1809,6 +1809,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="A97:C97"/>
+    <mergeCell ref="A119:C119"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C5"/>
+    <mergeCell ref="A6:C6"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B15:C15"/>
     <mergeCell ref="A108:C108"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="A130:C130"/>
@@ -1825,23 +1842,6 @@
     <mergeCell ref="A64:C64"/>
     <mergeCell ref="A75:C75"/>
     <mergeCell ref="A86:C86"/>
-    <mergeCell ref="A97:C97"/>
-    <mergeCell ref="A119:C119"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B12:C12"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>